<commit_message>
Correccion cuando el que entra no tiene Rutas
</commit_message>
<xml_diff>
--- a/Fleet Paqueteria.xlsx
+++ b/Fleet Paqueteria.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Flutter\fleetdeliveryapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B672EF64-AE4A-40D1-A1DC-C44CDE090C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647A0E1F-BE33-488C-B5F9-4BFF6EB5FE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9ACF8A49-EE6E-47DE-9CD9-2B198662CB92}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3819" uniqueCount="1461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3818" uniqueCount="1460">
   <si>
     <t>Server=www.fleetsa.com.ar;Database=ObrasOT;User Id=gaos;password=gaosfleetb4a$</t>
   </si>
@@ -3507,30 +3507,12 @@
     <t>RECHAZADO</t>
   </si>
   <si>
-    <t xml:space="preserve"> where IdRuta=1569 or IdRuta=1570 or IdRuta=1599</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> where NroRuta=1569 or NroRuta=1570 or NroRuta=1599</t>
-  </si>
-  <si>
     <t>SELECT ID, IdRuta, IdEnvio, Tag, Secuencia, Leyenda, Latitud, Longitud, IconoPropio, IDmapa, Distancia, Tiempo, Estado, Fecha, Hora, IdMotivo, NotaChofer, NuevoOrden, IDCabCertificacion, IdLiquidacionFletero, Turno</t>
   </si>
   <si>
     <t>FROM     p_Paradas</t>
   </si>
   <si>
-    <t>WHERE  (IdRuta = 1569 OR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                  IdRuta = 1570 OR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                  IdRuta = 1599) AND (IdEnvio &gt; 0)</t>
-  </si>
-  <si>
-    <t>ORDER BY IdEnvio</t>
-  </si>
-  <si>
     <t xml:space="preserve">SELECT ID, IDPROVEEDOR, AGENCIANR, ESTADO, ENVIA, RUTA, ORDENID, FECHA, HORA, IMEI, TRANSPORTE, CONTRATO, TITULAR, DNI, DOMICILIO, CP, LATITUD, LONGITUD, AUTORIZADO, OBSERVACIONES, IDCabCertificacion, </t>
   </si>
   <si>
@@ -4423,6 +4405,21 @@
   </si>
   <si>
     <t>SEGUIMIENTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> where IdRuta=1599 or IdRuta=4491</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> where NroRuta=1599 or NroRuta=4491</t>
+  </si>
+  <si>
+    <t>ORDER BY IdRuta, Secuencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  IdRuta = 4491)</t>
+  </si>
+  <si>
+    <t>WHERE  (IdRuta = 1599 OR</t>
   </si>
 </sst>
 </file>
@@ -4692,7 +4689,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4721,7 +4718,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4737,9 +4733,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -5217,7 +5210,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>1420</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -5257,19 +5250,19 @@
       <c r="L2" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="M2" s="48" t="s">
+      <c r="M2" s="46" t="s">
         <v>570</v>
       </c>
-      <c r="N2" s="48" t="s">
+      <c r="N2" s="46" t="s">
         <v>614</v>
       </c>
-      <c r="O2" s="48" t="s">
+      <c r="O2" s="46" t="s">
         <v>615</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="Q2" s="48" t="s">
+      <c r="Q2" s="46" t="s">
         <v>617</v>
       </c>
       <c r="R2" s="3" t="s">
@@ -5286,13 +5279,13 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="49">
+      <c r="A3" s="47">
         <v>75026</v>
       </c>
       <c r="B3" s="2">
         <v>1570</v>
       </c>
-      <c r="C3" s="49">
+      <c r="C3" s="47">
         <v>1005265</v>
       </c>
       <c r="D3" s="2">
@@ -5302,7 +5295,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1367</v>
+        <v>1361</v>
       </c>
       <c r="G3" s="11">
         <v>-345287848</v>
@@ -5311,7 +5304,7 @@
         <v>-587677978</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>1368</v>
+        <v>1362</v>
       </c>
       <c r="K3" s="2">
         <v>2464</v>
@@ -5361,7 +5354,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>1369</v>
+        <v>1363</v>
       </c>
       <c r="G4" s="11">
         <v>-345447303</v>
@@ -5370,7 +5363,7 @@
         <v>-587616742</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>1370</v>
+        <v>1364</v>
       </c>
       <c r="K4" s="2">
         <v>1443</v>
@@ -5420,7 +5413,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>1371</v>
+        <v>1365</v>
       </c>
       <c r="G5" s="11">
         <v>-345108987</v>
@@ -5429,7 +5422,7 @@
         <v>-588115753</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>1372</v>
+        <v>1366</v>
       </c>
       <c r="K5" s="2">
         <v>3334</v>
@@ -5479,7 +5472,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>1373</v>
+        <v>1367</v>
       </c>
       <c r="G6" s="11">
         <v>-345439542</v>
@@ -5488,7 +5481,7 @@
         <v>-587588683</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>1374</v>
+        <v>1368</v>
       </c>
       <c r="K6" s="2">
         <v>345</v>
@@ -5538,7 +5531,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>1375</v>
+        <v>1369</v>
       </c>
       <c r="G7" s="11">
         <v>-344674957</v>
@@ -5547,7 +5540,7 @@
         <v>-587214744</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>1376</v>
+        <v>1370</v>
       </c>
       <c r="K7" s="2">
         <v>1742</v>
@@ -5597,7 +5590,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>1377</v>
+        <v>1371</v>
       </c>
       <c r="G8" s="11">
         <v>-345376125</v>
@@ -5606,7 +5599,7 @@
         <v>-587684367</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>1378</v>
+        <v>1372</v>
       </c>
       <c r="K8" s="2">
         <v>2452</v>
@@ -5656,7 +5649,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>1379</v>
+        <v>1373</v>
       </c>
       <c r="G9" s="11">
         <v>-345382794</v>
@@ -5665,7 +5658,7 @@
         <v>-587784271</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>1380</v>
+        <v>1374</v>
       </c>
       <c r="K9" s="2">
         <v>1156</v>
@@ -5715,7 +5708,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>1381</v>
+        <v>1375</v>
       </c>
       <c r="G10" s="11">
         <v>-344995726</v>
@@ -5724,7 +5717,7 @@
         <v>-587194224</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>1382</v>
+        <v>1376</v>
       </c>
       <c r="K10" s="2">
         <v>3216</v>
@@ -5774,7 +5767,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>1383</v>
+        <v>1377</v>
       </c>
       <c r="G11" s="11">
         <v>-344945856</v>
@@ -5783,7 +5776,7 @@
         <v>-587236774</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>1384</v>
+        <v>1378</v>
       </c>
       <c r="K11" s="2">
         <v>914</v>
@@ -5833,7 +5826,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>1385</v>
+        <v>1379</v>
       </c>
       <c r="G12" s="11">
         <v>-344975134</v>
@@ -5842,7 +5835,7 @@
         <v>-588034897</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>1386</v>
+        <v>1380</v>
       </c>
       <c r="K12" s="2">
         <v>3938</v>
@@ -5892,7 +5885,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>1387</v>
+        <v>1381</v>
       </c>
       <c r="G13" s="11">
         <v>-345306090</v>
@@ -5901,7 +5894,7 @@
         <v>-587632754</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>1388</v>
+        <v>1382</v>
       </c>
       <c r="K13" s="2">
         <v>1343</v>
@@ -5951,7 +5944,7 @@
         <v>8</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>1389</v>
+        <v>1383</v>
       </c>
       <c r="G14" s="11">
         <v>-344760783</v>
@@ -5960,7 +5953,7 @@
         <v>-587352971</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>1390</v>
+        <v>1384</v>
       </c>
       <c r="K14" s="2">
         <v>3280</v>
@@ -6010,7 +6003,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>1391</v>
+        <v>1385</v>
       </c>
       <c r="G15" s="11">
         <v>-345192488</v>
@@ -6019,7 +6012,7 @@
         <v>-587228082</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>1392</v>
+        <v>1386</v>
       </c>
       <c r="K15" s="2">
         <v>3938</v>
@@ -6069,7 +6062,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>1393</v>
+        <v>1387</v>
       </c>
       <c r="G16" s="11">
         <v>-345082388</v>
@@ -6078,7 +6071,7 @@
         <v>-587890180</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>1394</v>
+        <v>1388</v>
       </c>
       <c r="K16" s="2">
         <v>880</v>
@@ -6128,7 +6121,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>1395</v>
+        <v>1389</v>
       </c>
       <c r="G17" s="11">
         <v>-345210608</v>
@@ -6137,7 +6130,7 @@
         <v>-588067114</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>1396</v>
+        <v>1390</v>
       </c>
       <c r="K17" s="2">
         <v>2930</v>
@@ -6187,7 +6180,7 @@
         <v>5</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>1397</v>
+        <v>1391</v>
       </c>
       <c r="G18" s="11">
         <v>-345418555</v>
@@ -6196,7 +6189,7 @@
         <v>-587878331</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>1398</v>
+        <v>1392</v>
       </c>
       <c r="K18" s="2">
         <v>5047</v>
@@ -6246,7 +6239,7 @@
         <v>12</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>1399</v>
+        <v>1393</v>
       </c>
       <c r="G19" s="11">
         <v>-345257592</v>
@@ -6255,7 +6248,7 @@
         <v>-587414509</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>1400</v>
+        <v>1394</v>
       </c>
       <c r="K19" s="2">
         <v>2222</v>
@@ -6289,13 +6282,13 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" s="50">
+      <c r="A20" s="48">
         <v>75006</v>
       </c>
       <c r="B20" s="2">
         <v>1569</v>
       </c>
-      <c r="C20" s="50">
+      <c r="C20" s="48">
         <v>1005283</v>
       </c>
       <c r="D20" s="2">
@@ -6305,7 +6298,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>1401</v>
+        <v>1395</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>32</v>
@@ -6314,7 +6307,7 @@
         <v>32</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>1402</v>
+        <v>1396</v>
       </c>
       <c r="K20" s="2">
         <v>4620</v>
@@ -6364,7 +6357,7 @@
         <v>11</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>1403</v>
+        <v>1397</v>
       </c>
       <c r="G21" s="11">
         <v>-345391599</v>
@@ -6373,7 +6366,7 @@
         <v>-587562401</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>1404</v>
+        <v>1398</v>
       </c>
       <c r="K21" s="2">
         <v>833</v>
@@ -6423,7 +6416,7 @@
         <v>9</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>1405</v>
+        <v>1399</v>
       </c>
       <c r="G22" s="11">
         <v>-344692630</v>
@@ -6432,7 +6425,7 @@
         <v>-587357355</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>1406</v>
+        <v>1400</v>
       </c>
       <c r="K22" s="2">
         <v>1216</v>
@@ -6482,7 +6475,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>1407</v>
+        <v>1401</v>
       </c>
       <c r="G23" s="11">
         <v>-344685610</v>
@@ -6491,7 +6484,7 @@
         <v>-587620727</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>1408</v>
+        <v>1402</v>
       </c>
       <c r="K23" s="2">
         <v>5364</v>
@@ -6541,7 +6534,7 @@
         <v>3</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>1409</v>
+        <v>1403</v>
       </c>
       <c r="G24" s="11">
         <v>-345005660</v>
@@ -6550,7 +6543,7 @@
         <v>-587988324</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>1410</v>
+        <v>1404</v>
       </c>
       <c r="K24" s="2">
         <v>588</v>
@@ -6600,7 +6593,7 @@
         <v>8</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>1331</v>
+        <v>1325</v>
       </c>
       <c r="G25" s="11">
         <v>-346077811</v>
@@ -6609,7 +6602,7 @@
         <v>-587793879</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>1411</v>
+        <v>1405</v>
       </c>
       <c r="K25" s="2">
         <v>1866</v>
@@ -6659,7 +6652,7 @@
         <v>7</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>1338</v>
+        <v>1332</v>
       </c>
       <c r="G26" s="11">
         <v>-346026054</v>
@@ -6668,7 +6661,7 @@
         <v>-587987894</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>1412</v>
+        <v>1406</v>
       </c>
       <c r="K26" s="2">
         <v>8708</v>
@@ -6718,7 +6711,7 @@
         <v>5</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>1341</v>
+        <v>1335</v>
       </c>
       <c r="G27" s="11">
         <v>-344971513</v>
@@ -6727,7 +6720,7 @@
         <v>-588031755</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>1413</v>
+        <v>1407</v>
       </c>
       <c r="K27" s="2">
         <v>3520</v>
@@ -6777,7 +6770,7 @@
         <v>6</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>1346</v>
+        <v>1340</v>
       </c>
       <c r="G28" s="11">
         <v>-345249159</v>
@@ -6786,7 +6779,7 @@
         <v>-588108441</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>1414</v>
+        <v>1408</v>
       </c>
       <c r="K28" s="2">
         <v>3166</v>
@@ -6836,7 +6829,7 @@
         <v>3</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>1351</v>
+        <v>1345</v>
       </c>
       <c r="G29" s="11">
         <v>-345090442</v>
@@ -6845,7 +6838,7 @@
         <v>-587674604</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>1415</v>
+        <v>1409</v>
       </c>
       <c r="K29" s="2">
         <v>2992</v>
@@ -6895,7 +6888,7 @@
         <v>9</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>1354</v>
+        <v>1348</v>
       </c>
       <c r="G30" s="11">
         <v>-346210840</v>
@@ -6904,7 +6897,7 @@
         <v>-588040839</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>1416</v>
+        <v>1410</v>
       </c>
       <c r="K30" s="2">
         <v>2701</v>
@@ -6954,7 +6947,7 @@
         <v>2</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>1357</v>
+        <v>1351</v>
       </c>
       <c r="G31" s="11">
         <v>-345170228</v>
@@ -6963,7 +6956,7 @@
         <v>-587855437</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>1417</v>
+        <v>1411</v>
       </c>
       <c r="K31" s="2">
         <v>3582</v>
@@ -7013,7 +7006,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>1360</v>
+        <v>1354</v>
       </c>
       <c r="G32" s="11">
         <v>-345220599</v>
@@ -7022,7 +7015,7 @@
         <v>-587881878</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>1418</v>
+        <v>1412</v>
       </c>
       <c r="K32" s="2">
         <v>4418</v>
@@ -7072,7 +7065,7 @@
         <v>4</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>1363</v>
+        <v>1357</v>
       </c>
       <c r="G33" s="11">
         <v>-344962519</v>
@@ -7081,7 +7074,7 @@
         <v>-587647798</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>1419</v>
+        <v>1413</v>
       </c>
       <c r="K33" s="2">
         <v>1443</v>
@@ -7116,7 +7109,7 @@
     </row>
     <row r="35" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>1421</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="36" spans="1:76" x14ac:dyDescent="0.2">
@@ -7129,7 +7122,7 @@
       <c r="C36" s="3" t="s">
         <v>730</v>
       </c>
-      <c r="D36" s="48" t="s">
+      <c r="D36" s="46" t="s">
         <v>731</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -7216,7 +7209,7 @@
       <c r="AF36" s="3" t="s">
         <v>756</v>
       </c>
-      <c r="AG36" s="48" t="s">
+      <c r="AG36" s="46" t="s">
         <v>757</v>
       </c>
       <c r="AH36" s="3" t="s">
@@ -7276,7 +7269,7 @@
       <c r="AZ36" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="BA36" s="48" t="s">
+      <c r="BA36" s="46" t="s">
         <v>776</v>
       </c>
       <c r="BB36" s="3" t="s">
@@ -7309,10 +7302,10 @@
       <c r="BK36" s="3" t="s">
         <v>786</v>
       </c>
-      <c r="BL36" s="48" t="s">
+      <c r="BL36" s="46" t="s">
         <v>787</v>
       </c>
-      <c r="BM36" s="48" t="s">
+      <c r="BM36" s="46" t="s">
         <v>788</v>
       </c>
       <c r="BN36" s="3" t="s">
@@ -7340,17 +7333,17 @@
         <v>795</v>
       </c>
       <c r="BV36" s="3" t="s">
-        <v>1235</v>
+        <v>1229</v>
       </c>
       <c r="BW36" s="3" t="s">
-        <v>1236</v>
+        <v>1230</v>
       </c>
       <c r="BX36" s="3" t="s">
-        <v>1237</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="37" spans="1:76" x14ac:dyDescent="0.2">
-      <c r="A37" s="49">
+      <c r="A37" s="47">
         <v>1005265</v>
       </c>
       <c r="B37" s="2">
@@ -7381,13 +7374,13 @@
         <v>32</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>1238</v>
+        <v>1232</v>
       </c>
       <c r="N37" s="2">
         <v>20000004</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>1239</v>
+        <v>1233</v>
       </c>
       <c r="P37" s="2">
         <v>1665</v>
@@ -7414,7 +7407,7 @@
         <v>446</v>
       </c>
       <c r="X37" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y37" s="2" t="s">
         <v>32</v>
@@ -7423,13 +7416,13 @@
         <v>44574</v>
       </c>
       <c r="AA37" s="2" t="s">
-        <v>1241</v>
+        <v>1235</v>
       </c>
       <c r="AB37" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC37" s="2" t="s">
-        <v>1242</v>
+        <v>1236</v>
       </c>
       <c r="AD37" s="2" t="s">
         <v>815</v>
@@ -7480,7 +7473,7 @@
         <v>0</v>
       </c>
       <c r="AZ37" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA37" s="12">
         <v>44729</v>
@@ -7563,13 +7556,13 @@
         <v>32</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>1244</v>
+        <v>1238</v>
       </c>
       <c r="N38" s="2">
         <v>20000008</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>1245</v>
+        <v>1239</v>
       </c>
       <c r="P38" s="2">
         <v>1665</v>
@@ -7596,7 +7589,7 @@
         <v>446</v>
       </c>
       <c r="X38" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y38" s="2" t="s">
         <v>32</v>
@@ -7605,13 +7598,13 @@
         <v>44574</v>
       </c>
       <c r="AA38" s="2" t="s">
-        <v>1246</v>
+        <v>1240</v>
       </c>
       <c r="AB38" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC38" s="2" t="s">
-        <v>1247</v>
+        <v>1241</v>
       </c>
       <c r="AD38" s="2" t="s">
         <v>815</v>
@@ -7662,7 +7655,7 @@
         <v>0</v>
       </c>
       <c r="AZ38" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA38" s="12">
         <v>44729</v>
@@ -7745,13 +7738,13 @@
         <v>32</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>1248</v>
+        <v>1242</v>
       </c>
       <c r="N39" s="2">
         <v>20000001</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>1249</v>
+        <v>1243</v>
       </c>
       <c r="P39" s="2">
         <v>1615</v>
@@ -7778,7 +7771,7 @@
         <v>446</v>
       </c>
       <c r="X39" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y39" s="2" t="s">
         <v>32</v>
@@ -7787,16 +7780,16 @@
         <v>44574</v>
       </c>
       <c r="AA39" s="2" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="AB39" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC39" s="2" t="s">
-        <v>1251</v>
+        <v>1245</v>
       </c>
       <c r="AD39" s="2" t="s">
-        <v>1252</v>
+        <v>1246</v>
       </c>
       <c r="AE39" s="2" t="s">
         <v>32</v>
@@ -7844,7 +7837,7 @@
         <v>0</v>
       </c>
       <c r="AZ39" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA39" s="12">
         <v>44729</v>
@@ -7927,13 +7920,13 @@
         <v>32</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>1253</v>
+        <v>1247</v>
       </c>
       <c r="N40" s="2">
         <v>20000005</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>1254</v>
+        <v>1248</v>
       </c>
       <c r="P40" s="2">
         <v>1665</v>
@@ -7960,7 +7953,7 @@
         <v>446</v>
       </c>
       <c r="X40" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y40" s="2" t="s">
         <v>32</v>
@@ -7969,13 +7962,13 @@
         <v>44574</v>
       </c>
       <c r="AA40" s="2" t="s">
-        <v>1255</v>
+        <v>1249</v>
       </c>
       <c r="AB40" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC40" s="2" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="AD40" s="2" t="s">
         <v>815</v>
@@ -8026,7 +8019,7 @@
         <v>0</v>
       </c>
       <c r="AZ40" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA40" s="12">
         <v>44729</v>
@@ -8109,13 +8102,13 @@
         <v>32</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>1257</v>
+        <v>1251</v>
       </c>
       <c r="N41" s="2">
         <v>20000007</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>1258</v>
+        <v>1252</v>
       </c>
       <c r="P41" s="2">
         <v>1615</v>
@@ -8139,7 +8132,7 @@
         <v>446</v>
       </c>
       <c r="X41" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y41" s="2" t="s">
         <v>32</v>
@@ -8148,16 +8141,16 @@
         <v>44574</v>
       </c>
       <c r="AA41" s="2" t="s">
-        <v>1259</v>
+        <v>1253</v>
       </c>
       <c r="AB41" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC41" s="2" t="s">
-        <v>1260</v>
+        <v>1254</v>
       </c>
       <c r="AD41" s="2" t="s">
-        <v>1252</v>
+        <v>1246</v>
       </c>
       <c r="AE41" s="2" t="s">
         <v>32</v>
@@ -8205,7 +8198,7 @@
         <v>0</v>
       </c>
       <c r="AZ41" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA41" s="12">
         <v>44729</v>
@@ -8288,13 +8281,13 @@
         <v>32</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>1261</v>
+        <v>1255</v>
       </c>
       <c r="N42" s="2">
         <v>20000010</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>1262</v>
+        <v>1256</v>
       </c>
       <c r="P42" s="2">
         <v>1665</v>
@@ -8321,7 +8314,7 @@
         <v>446</v>
       </c>
       <c r="X42" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y42" s="2" t="s">
         <v>32</v>
@@ -8330,13 +8323,13 @@
         <v>44574</v>
       </c>
       <c r="AA42" s="2" t="s">
-        <v>1263</v>
+        <v>1257</v>
       </c>
       <c r="AB42" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC42" s="2" t="s">
-        <v>1264</v>
+        <v>1258</v>
       </c>
       <c r="AD42" s="2" t="s">
         <v>815</v>
@@ -8387,7 +8380,7 @@
         <v>0</v>
       </c>
       <c r="AZ42" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA42" s="12">
         <v>44729</v>
@@ -8470,13 +8463,13 @@
         <v>32</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>1265</v>
+        <v>1259</v>
       </c>
       <c r="N43" s="2">
         <v>20000002</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>1266</v>
+        <v>1260</v>
       </c>
       <c r="P43" s="2">
         <v>1665</v>
@@ -8503,7 +8496,7 @@
         <v>446</v>
       </c>
       <c r="X43" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y43" s="2" t="s">
         <v>32</v>
@@ -8512,13 +8505,13 @@
         <v>44574</v>
       </c>
       <c r="AA43" s="2" t="s">
-        <v>1267</v>
+        <v>1261</v>
       </c>
       <c r="AB43" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC43" s="2" t="s">
-        <v>1268</v>
+        <v>1262</v>
       </c>
       <c r="AD43" s="2" t="s">
         <v>815</v>
@@ -8569,7 +8562,7 @@
         <v>0</v>
       </c>
       <c r="AZ43" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA43" s="12">
         <v>44729</v>
@@ -8652,13 +8645,13 @@
         <v>32</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>1269</v>
+        <v>1263</v>
       </c>
       <c r="N44" s="2">
         <v>20000020</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>1270</v>
+        <v>1264</v>
       </c>
       <c r="P44" s="2">
         <v>1665</v>
@@ -8682,7 +8675,7 @@
         <v>446</v>
       </c>
       <c r="X44" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y44" s="2" t="s">
         <v>32</v>
@@ -8691,13 +8684,13 @@
         <v>44574</v>
       </c>
       <c r="AA44" s="2" t="s">
-        <v>1271</v>
+        <v>1265</v>
       </c>
       <c r="AB44" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC44" s="2" t="s">
-        <v>1272</v>
+        <v>1266</v>
       </c>
       <c r="AD44" s="2" t="s">
         <v>815</v>
@@ -8748,7 +8741,7 @@
         <v>0</v>
       </c>
       <c r="AZ44" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA44" s="12">
         <v>44729</v>
@@ -8831,13 +8824,13 @@
         <v>32</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>1273</v>
+        <v>1267</v>
       </c>
       <c r="N45" s="2">
         <v>20000014</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>1274</v>
+        <v>1268</v>
       </c>
       <c r="P45" s="2">
         <v>1665</v>
@@ -8861,7 +8854,7 @@
         <v>446</v>
       </c>
       <c r="X45" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y45" s="2" t="s">
         <v>32</v>
@@ -8870,13 +8863,13 @@
         <v>44574</v>
       </c>
       <c r="AA45" s="2" t="s">
-        <v>1275</v>
+        <v>1269</v>
       </c>
       <c r="AB45" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC45" s="2" t="s">
-        <v>1276</v>
+        <v>1270</v>
       </c>
       <c r="AD45" s="2" t="s">
         <v>815</v>
@@ -8927,7 +8920,7 @@
         <v>0</v>
       </c>
       <c r="AZ45" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA45" s="12">
         <v>44729</v>
@@ -9010,13 +9003,13 @@
         <v>32</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>1277</v>
+        <v>1271</v>
       </c>
       <c r="N46" s="2">
         <v>20000012</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>1278</v>
+        <v>1272</v>
       </c>
       <c r="P46" s="2">
         <v>1665</v>
@@ -9043,7 +9036,7 @@
         <v>446</v>
       </c>
       <c r="X46" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y46" s="2" t="s">
         <v>32</v>
@@ -9052,13 +9045,13 @@
         <v>44574</v>
       </c>
       <c r="AA46" s="2" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="AB46" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC46" s="2" t="s">
-        <v>1280</v>
+        <v>1274</v>
       </c>
       <c r="AD46" s="2" t="s">
         <v>815</v>
@@ -9109,7 +9102,7 @@
         <v>0</v>
       </c>
       <c r="AZ46" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA46" s="12">
         <v>44729</v>
@@ -9192,13 +9185,13 @@
         <v>32</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>1281</v>
+        <v>1275</v>
       </c>
       <c r="N47" s="2">
         <v>20000021</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>1282</v>
+        <v>1276</v>
       </c>
       <c r="P47" s="2">
         <v>1665</v>
@@ -9222,7 +9215,7 @@
         <v>446</v>
       </c>
       <c r="X47" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y47" s="2" t="s">
         <v>32</v>
@@ -9231,13 +9224,13 @@
         <v>44574</v>
       </c>
       <c r="AA47" s="2" t="s">
-        <v>1283</v>
+        <v>1277</v>
       </c>
       <c r="AB47" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC47" s="2" t="s">
-        <v>1284</v>
+        <v>1278</v>
       </c>
       <c r="AD47" s="2" t="s">
         <v>815</v>
@@ -9288,7 +9281,7 @@
         <v>0</v>
       </c>
       <c r="AZ47" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA47" s="12">
         <v>44729</v>
@@ -9371,13 +9364,13 @@
         <v>32</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>1285</v>
+        <v>1279</v>
       </c>
       <c r="N48" s="2">
         <v>20000017</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>1286</v>
+        <v>1280</v>
       </c>
       <c r="P48" s="2">
         <v>1665</v>
@@ -9401,7 +9394,7 @@
         <v>446</v>
       </c>
       <c r="X48" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y48" s="2" t="s">
         <v>32</v>
@@ -9410,13 +9403,13 @@
         <v>44574</v>
       </c>
       <c r="AA48" s="2" t="s">
-        <v>1287</v>
+        <v>1281</v>
       </c>
       <c r="AB48" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC48" s="2" t="s">
-        <v>1288</v>
+        <v>1282</v>
       </c>
       <c r="AD48" s="2" t="s">
         <v>815</v>
@@ -9467,7 +9460,7 @@
         <v>0</v>
       </c>
       <c r="AZ48" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA48" s="12">
         <v>44729</v>
@@ -9550,13 +9543,13 @@
         <v>32</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>1289</v>
+        <v>1283</v>
       </c>
       <c r="N49" s="2">
         <v>20000013</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>1290</v>
+        <v>1284</v>
       </c>
       <c r="P49" s="2">
         <v>1665</v>
@@ -9580,7 +9573,7 @@
         <v>446</v>
       </c>
       <c r="X49" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y49" s="2" t="s">
         <v>32</v>
@@ -9589,13 +9582,13 @@
         <v>44574</v>
       </c>
       <c r="AA49" s="2" t="s">
-        <v>1291</v>
+        <v>1285</v>
       </c>
       <c r="AB49" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC49" s="2" t="s">
-        <v>1292</v>
+        <v>1286</v>
       </c>
       <c r="AD49" s="2" t="s">
         <v>815</v>
@@ -9646,7 +9639,7 @@
         <v>0</v>
       </c>
       <c r="AZ49" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA49" s="12">
         <v>44729</v>
@@ -9729,13 +9722,13 @@
         <v>32</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>1293</v>
+        <v>1287</v>
       </c>
       <c r="N50" s="2">
         <v>20000005</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>1294</v>
+        <v>1288</v>
       </c>
       <c r="P50" s="2">
         <v>1665</v>
@@ -9759,7 +9752,7 @@
         <v>446</v>
       </c>
       <c r="X50" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y50" s="2" t="s">
         <v>32</v>
@@ -9768,13 +9761,13 @@
         <v>44574</v>
       </c>
       <c r="AA50" s="2" t="s">
-        <v>1295</v>
+        <v>1289</v>
       </c>
       <c r="AB50" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC50" s="2" t="s">
-        <v>1296</v>
+        <v>1290</v>
       </c>
       <c r="AD50" s="2" t="s">
         <v>815</v>
@@ -9825,7 +9818,7 @@
         <v>0</v>
       </c>
       <c r="AZ50" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA50" s="12">
         <v>44729</v>
@@ -9908,13 +9901,13 @@
         <v>32</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="N51" s="2">
         <v>20000022</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>1298</v>
+        <v>1292</v>
       </c>
       <c r="P51" s="2">
         <v>1665</v>
@@ -9941,7 +9934,7 @@
         <v>446</v>
       </c>
       <c r="X51" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y51" s="2" t="s">
         <v>32</v>
@@ -9950,13 +9943,13 @@
         <v>44574</v>
       </c>
       <c r="AA51" s="2" t="s">
-        <v>1299</v>
+        <v>1293</v>
       </c>
       <c r="AB51" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC51" s="2" t="s">
-        <v>1300</v>
+        <v>1294</v>
       </c>
       <c r="AD51" s="2" t="s">
         <v>815</v>
@@ -10007,7 +10000,7 @@
         <v>0</v>
       </c>
       <c r="AZ51" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA51" s="12">
         <v>44729</v>
@@ -10090,13 +10083,13 @@
         <v>32</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>1301</v>
+        <v>1295</v>
       </c>
       <c r="N52" s="2">
         <v>20000018</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>1302</v>
+        <v>1296</v>
       </c>
       <c r="P52" s="2">
         <v>1665</v>
@@ -10123,7 +10116,7 @@
         <v>446</v>
       </c>
       <c r="X52" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y52" s="2" t="s">
         <v>32</v>
@@ -10132,13 +10125,13 @@
         <v>44574</v>
       </c>
       <c r="AA52" s="2" t="s">
-        <v>1303</v>
+        <v>1297</v>
       </c>
       <c r="AB52" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC52" s="2" t="s">
-        <v>1304</v>
+        <v>1298</v>
       </c>
       <c r="AD52" s="2" t="s">
         <v>815</v>
@@ -10189,7 +10182,7 @@
         <v>0</v>
       </c>
       <c r="AZ52" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA52" s="12">
         <v>44729</v>
@@ -10272,13 +10265,13 @@
         <v>32</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>1305</v>
+        <v>1299</v>
       </c>
       <c r="N53" s="2">
         <v>20000015</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>1306</v>
+        <v>1300</v>
       </c>
       <c r="P53" s="2">
         <v>1665</v>
@@ -10305,7 +10298,7 @@
         <v>446</v>
       </c>
       <c r="X53" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y53" s="2" t="s">
         <v>32</v>
@@ -10314,13 +10307,13 @@
         <v>44574</v>
       </c>
       <c r="AA53" s="2" t="s">
-        <v>1307</v>
+        <v>1301</v>
       </c>
       <c r="AB53" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC53" s="2" t="s">
-        <v>1308</v>
+        <v>1302</v>
       </c>
       <c r="AD53" s="2" t="s">
         <v>815</v>
@@ -10371,7 +10364,7 @@
         <v>0</v>
       </c>
       <c r="AZ53" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA53" s="12">
         <v>44729</v>
@@ -10423,7 +10416,7 @@
       </c>
     </row>
     <row r="54" spans="1:76" x14ac:dyDescent="0.2">
-      <c r="A54" s="50">
+      <c r="A54" s="48">
         <v>1005283</v>
       </c>
       <c r="B54" s="2">
@@ -10454,13 +10447,13 @@
         <v>32</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>1309</v>
+        <v>1303</v>
       </c>
       <c r="N54" s="2">
         <v>20000009</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>1310</v>
+        <v>1304</v>
       </c>
       <c r="P54" s="2">
         <v>1665</v>
@@ -10484,7 +10477,7 @@
         <v>446</v>
       </c>
       <c r="X54" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y54" s="2" t="s">
         <v>32</v>
@@ -10493,13 +10486,13 @@
         <v>44574</v>
       </c>
       <c r="AA54" s="2" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="AB54" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC54" s="2" t="s">
-        <v>1312</v>
+        <v>1306</v>
       </c>
       <c r="AD54" s="2" t="s">
         <v>815</v>
@@ -10550,7 +10543,7 @@
         <v>0</v>
       </c>
       <c r="AZ54" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA54" s="12">
         <v>44729</v>
@@ -10633,13 +10626,13 @@
         <v>32</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>1313</v>
+        <v>1307</v>
       </c>
       <c r="N55" s="2">
         <v>20000019</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>1314</v>
+        <v>1308</v>
       </c>
       <c r="P55" s="2">
         <v>1665</v>
@@ -10666,7 +10659,7 @@
         <v>446</v>
       </c>
       <c r="X55" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y55" s="2" t="s">
         <v>32</v>
@@ -10675,13 +10668,13 @@
         <v>44574</v>
       </c>
       <c r="AA55" s="2" t="s">
-        <v>1315</v>
+        <v>1309</v>
       </c>
       <c r="AB55" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC55" s="2" t="s">
-        <v>1316</v>
+        <v>1310</v>
       </c>
       <c r="AD55" s="2" t="s">
         <v>815</v>
@@ -10732,7 +10725,7 @@
         <v>0</v>
       </c>
       <c r="AZ55" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA55" s="12">
         <v>44729</v>
@@ -10815,13 +10808,13 @@
         <v>32</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="N56" s="2">
         <v>20000016</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="P56" s="2">
         <v>1665</v>
@@ -10845,7 +10838,7 @@
         <v>446</v>
       </c>
       <c r="X56" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y56" s="2" t="s">
         <v>32</v>
@@ -10854,13 +10847,13 @@
         <v>44574</v>
       </c>
       <c r="AA56" s="2" t="s">
-        <v>1319</v>
+        <v>1313</v>
       </c>
       <c r="AB56" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC56" s="2" t="s">
-        <v>1320</v>
+        <v>1314</v>
       </c>
       <c r="AD56" s="2" t="s">
         <v>815</v>
@@ -10911,7 +10904,7 @@
         <v>0</v>
       </c>
       <c r="AZ56" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA56" s="12">
         <v>44729</v>
@@ -10994,13 +10987,13 @@
         <v>32</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>1321</v>
+        <v>1315</v>
       </c>
       <c r="N57" s="2">
         <v>20000024</v>
       </c>
       <c r="O57" s="2" t="s">
-        <v>1322</v>
+        <v>1316</v>
       </c>
       <c r="P57" s="2">
         <v>1665</v>
@@ -11024,7 +11017,7 @@
         <v>446</v>
       </c>
       <c r="X57" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y57" s="2" t="s">
         <v>32</v>
@@ -11033,13 +11026,13 @@
         <v>44574</v>
       </c>
       <c r="AA57" s="2" t="s">
-        <v>1323</v>
+        <v>1317</v>
       </c>
       <c r="AB57" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC57" s="2" t="s">
-        <v>1324</v>
+        <v>1318</v>
       </c>
       <c r="AD57" s="2" t="s">
         <v>815</v>
@@ -11090,7 +11083,7 @@
         <v>0</v>
       </c>
       <c r="AZ57" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA57" s="12">
         <v>44729</v>
@@ -11173,13 +11166,13 @@
         <v>32</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>1325</v>
+        <v>1319</v>
       </c>
       <c r="N58" s="2">
         <v>20000026</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>1326</v>
+        <v>1320</v>
       </c>
       <c r="P58" s="2">
         <v>1665</v>
@@ -11206,7 +11199,7 @@
         <v>446</v>
       </c>
       <c r="X58" s="2" t="s">
-        <v>1240</v>
+        <v>1234</v>
       </c>
       <c r="Y58" s="2" t="s">
         <v>32</v>
@@ -11215,13 +11208,13 @@
         <v>44574</v>
       </c>
       <c r="AA58" s="2" t="s">
-        <v>1327</v>
+        <v>1321</v>
       </c>
       <c r="AB58" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC58" s="2" t="s">
-        <v>1328</v>
+        <v>1322</v>
       </c>
       <c r="AD58" s="2" t="s">
         <v>815</v>
@@ -11272,7 +11265,7 @@
         <v>0</v>
       </c>
       <c r="AZ58" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA58" s="12">
         <v>44729</v>
@@ -11355,13 +11348,13 @@
         <v>32</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>1331</v>
+        <v>1325</v>
       </c>
       <c r="P59" s="2">
         <v>1744</v>
@@ -11388,7 +11381,7 @@
         <v>446</v>
       </c>
       <c r="X59" s="2" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="Y59" s="12">
         <v>44578</v>
@@ -11397,16 +11390,16 @@
         <v>44578</v>
       </c>
       <c r="AA59" s="2" t="s">
-        <v>1333</v>
+        <v>1327</v>
       </c>
       <c r="AB59" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC59" s="2" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="AD59" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="AE59" s="2" t="s">
         <v>32</v>
@@ -11445,7 +11438,7 @@
         <v>0</v>
       </c>
       <c r="AU59" s="2" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="AV59" s="12">
         <v>44578</v>
@@ -11454,7 +11447,7 @@
         <v>0</v>
       </c>
       <c r="AZ59" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA59" s="12">
         <v>44729</v>
@@ -11537,13 +11530,13 @@
         <v>32</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>1337</v>
+        <v>1331</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="O60" s="2" t="s">
-        <v>1338</v>
+        <v>1332</v>
       </c>
       <c r="P60" s="2">
         <v>1744</v>
@@ -11570,7 +11563,7 @@
         <v>446</v>
       </c>
       <c r="X60" s="2" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="Y60" s="12">
         <v>44578</v>
@@ -11579,16 +11572,16 @@
         <v>44578</v>
       </c>
       <c r="AA60" s="2" t="s">
-        <v>1339</v>
+        <v>1333</v>
       </c>
       <c r="AB60" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC60" s="2" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="AD60" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="AE60" s="2" t="s">
         <v>32</v>
@@ -11627,7 +11620,7 @@
         <v>0</v>
       </c>
       <c r="AU60" s="2" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="AV60" s="12">
         <v>44578</v>
@@ -11636,7 +11629,7 @@
         <v>0</v>
       </c>
       <c r="AZ60" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA60" s="12">
         <v>44729</v>
@@ -11719,13 +11712,13 @@
         <v>32</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>1340</v>
+        <v>1334</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="O61" s="2" t="s">
-        <v>1341</v>
+        <v>1335</v>
       </c>
       <c r="P61" s="2">
         <v>1665</v>
@@ -11752,7 +11745,7 @@
         <v>446</v>
       </c>
       <c r="X61" s="2" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="Y61" s="12">
         <v>44578</v>
@@ -11761,16 +11754,16 @@
         <v>44578</v>
       </c>
       <c r="AA61" s="2" t="s">
-        <v>1342</v>
+        <v>1336</v>
       </c>
       <c r="AB61" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC61" s="2" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="AD61" s="2" t="s">
-        <v>1343</v>
+        <v>1337</v>
       </c>
       <c r="AE61" s="2" t="s">
         <v>32</v>
@@ -11809,7 +11802,7 @@
         <v>0</v>
       </c>
       <c r="AU61" s="2" t="s">
-        <v>1344</v>
+        <v>1338</v>
       </c>
       <c r="AV61" s="12">
         <v>44578</v>
@@ -11818,7 +11811,7 @@
         <v>0</v>
       </c>
       <c r="AZ61" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA61" s="12">
         <v>44729</v>
@@ -11901,13 +11894,13 @@
         <v>32</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>1345</v>
+        <v>1339</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="O62" s="2" t="s">
-        <v>1346</v>
+        <v>1340</v>
       </c>
       <c r="P62" s="2">
         <v>1744</v>
@@ -11934,7 +11927,7 @@
         <v>446</v>
       </c>
       <c r="X62" s="2" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="Y62" s="12">
         <v>44578</v>
@@ -11943,16 +11936,16 @@
         <v>44578</v>
       </c>
       <c r="AA62" s="2" t="s">
-        <v>1347</v>
+        <v>1341</v>
       </c>
       <c r="AB62" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC62" s="2" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="AD62" s="2" t="s">
-        <v>1348</v>
+        <v>1342</v>
       </c>
       <c r="AE62" s="2" t="s">
         <v>32</v>
@@ -11991,7 +11984,7 @@
         <v>0</v>
       </c>
       <c r="AU62" s="2" t="s">
-        <v>1349</v>
+        <v>1343</v>
       </c>
       <c r="AV62" s="12">
         <v>44578</v>
@@ -12000,7 +11993,7 @@
         <v>0</v>
       </c>
       <c r="AZ62" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA62" s="12">
         <v>44729</v>
@@ -12083,13 +12076,13 @@
         <v>32</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>1350</v>
+        <v>1344</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="O63" s="2" t="s">
-        <v>1351</v>
+        <v>1345</v>
       </c>
       <c r="P63" s="2">
         <v>1665</v>
@@ -12116,7 +12109,7 @@
         <v>446</v>
       </c>
       <c r="X63" s="2" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="Y63" s="12">
         <v>44578</v>
@@ -12125,16 +12118,16 @@
         <v>44578</v>
       </c>
       <c r="AA63" s="2" t="s">
-        <v>1352</v>
+        <v>1346</v>
       </c>
       <c r="AB63" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC63" s="2" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="AD63" s="2" t="s">
-        <v>1343</v>
+        <v>1337</v>
       </c>
       <c r="AE63" s="2" t="s">
         <v>32</v>
@@ -12173,7 +12166,7 @@
         <v>0</v>
       </c>
       <c r="AU63" s="2" t="s">
-        <v>1349</v>
+        <v>1343</v>
       </c>
       <c r="AV63" s="12">
         <v>44578</v>
@@ -12182,7 +12175,7 @@
         <v>0</v>
       </c>
       <c r="AZ63" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA63" s="12">
         <v>44729</v>
@@ -12265,13 +12258,13 @@
         <v>32</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>1353</v>
+        <v>1347</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="O64" s="2" t="s">
-        <v>1354</v>
+        <v>1348</v>
       </c>
       <c r="P64" s="2">
         <v>1743</v>
@@ -12298,7 +12291,7 @@
         <v>446</v>
       </c>
       <c r="X64" s="2" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="Y64" s="12">
         <v>44578</v>
@@ -12307,16 +12300,16 @@
         <v>44578</v>
       </c>
       <c r="AA64" s="2" t="s">
-        <v>1355</v>
+        <v>1349</v>
       </c>
       <c r="AB64" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC64" s="2" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="AD64" s="2" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="AE64" s="2" t="s">
         <v>32</v>
@@ -12355,7 +12348,7 @@
         <v>0</v>
       </c>
       <c r="AU64" s="2" t="s">
-        <v>1344</v>
+        <v>1338</v>
       </c>
       <c r="AV64" s="12">
         <v>44578</v>
@@ -12364,7 +12357,7 @@
         <v>0</v>
       </c>
       <c r="AZ64" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA64" s="12">
         <v>44729</v>
@@ -12447,13 +12440,13 @@
         <v>32</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>1356</v>
+        <v>1350</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="O65" s="2" t="s">
-        <v>1357</v>
+        <v>1351</v>
       </c>
       <c r="P65" s="2">
         <v>1665</v>
@@ -12480,7 +12473,7 @@
         <v>446</v>
       </c>
       <c r="X65" s="2" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="Y65" s="12">
         <v>44578</v>
@@ -12489,16 +12482,16 @@
         <v>44578</v>
       </c>
       <c r="AA65" s="2" t="s">
-        <v>1358</v>
+        <v>1352</v>
       </c>
       <c r="AB65" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC65" s="2" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="AD65" s="2" t="s">
-        <v>1343</v>
+        <v>1337</v>
       </c>
       <c r="AE65" s="2" t="s">
         <v>32</v>
@@ -12537,7 +12530,7 @@
         <v>0</v>
       </c>
       <c r="AU65" s="2" t="s">
-        <v>1344</v>
+        <v>1338</v>
       </c>
       <c r="AV65" s="12">
         <v>44578</v>
@@ -12546,7 +12539,7 @@
         <v>0</v>
       </c>
       <c r="AZ65" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA65" s="12">
         <v>44729</v>
@@ -12629,13 +12622,13 @@
         <v>32</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>1359</v>
+        <v>1353</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="O66" s="2" t="s">
-        <v>1360</v>
+        <v>1354</v>
       </c>
       <c r="P66" s="2">
         <v>1665</v>
@@ -12662,7 +12655,7 @@
         <v>446</v>
       </c>
       <c r="X66" s="2" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="Y66" s="12">
         <v>44578</v>
@@ -12671,16 +12664,16 @@
         <v>44578</v>
       </c>
       <c r="AA66" s="2" t="s">
-        <v>1361</v>
+        <v>1355</v>
       </c>
       <c r="AB66" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC66" s="2" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="AD66" s="2" t="s">
-        <v>1343</v>
+        <v>1337</v>
       </c>
       <c r="AE66" s="2" t="s">
         <v>32</v>
@@ -12719,7 +12712,7 @@
         <v>0</v>
       </c>
       <c r="AU66" s="2" t="s">
-        <v>1344</v>
+        <v>1338</v>
       </c>
       <c r="AV66" s="12">
         <v>44578</v>
@@ -12728,7 +12721,7 @@
         <v>0</v>
       </c>
       <c r="AZ66" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA66" s="12">
         <v>44729</v>
@@ -12811,13 +12804,13 @@
         <v>32</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>1362</v>
+        <v>1356</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="O67" s="2" t="s">
-        <v>1363</v>
+        <v>1357</v>
       </c>
       <c r="P67" s="2">
         <v>1665</v>
@@ -12844,7 +12837,7 @@
         <v>446</v>
       </c>
       <c r="X67" s="2" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="Y67" s="12">
         <v>44578</v>
@@ -12853,16 +12846,16 @@
         <v>44578</v>
       </c>
       <c r="AA67" s="2" t="s">
-        <v>1364</v>
+        <v>1358</v>
       </c>
       <c r="AB67" s="2" t="s">
         <v>835</v>
       </c>
       <c r="AC67" s="2" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="AD67" s="2" t="s">
-        <v>1343</v>
+        <v>1337</v>
       </c>
       <c r="AE67" s="2" t="s">
         <v>32</v>
@@ -12901,7 +12894,7 @@
         <v>0</v>
       </c>
       <c r="AU67" s="2" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="AV67" s="12">
         <v>44578</v>
@@ -12910,7 +12903,7 @@
         <v>0</v>
       </c>
       <c r="AZ67" s="2" t="s">
-        <v>1243</v>
+        <v>1237</v>
       </c>
       <c r="BA67" s="12">
         <v>44729</v>
@@ -12931,13 +12924,13 @@
         <v>0</v>
       </c>
       <c r="BH67" s="2" t="s">
-        <v>1365</v>
+        <v>1359</v>
       </c>
       <c r="BI67" s="2">
         <v>2</v>
       </c>
       <c r="BK67" s="2" t="s">
-        <v>1366</v>
+        <v>1360</v>
       </c>
       <c r="BL67" s="2">
         <v>0</v>
@@ -12969,7 +12962,7 @@
     </row>
     <row r="69" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>1460</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="70" spans="1:76" x14ac:dyDescent="0.2">
@@ -12977,16 +12970,16 @@
         <v>602</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>1422</v>
+        <v>1416</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>1423</v>
+        <v>1417</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>731</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>1424</v>
+        <v>1418</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>735</v>
@@ -12998,20 +12991,20 @@
         <v>747</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>1425</v>
+        <v>1419</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>1426</v>
+        <v>1420</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>1427</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="71" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>3629719</v>
       </c>
-      <c r="B71" s="49">
+      <c r="B71" s="47">
         <v>1005265</v>
       </c>
       <c r="C71" s="2">
@@ -13023,17 +13016,17 @@
       <c r="E71" s="2">
         <v>446</v>
       </c>
-      <c r="F71" s="49">
+      <c r="F71" s="47">
         <v>80890</v>
       </c>
       <c r="G71" s="13">
         <v>0.7895833333333333</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>1429</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="72" spans="1:76" x14ac:dyDescent="0.2">
@@ -13059,10 +13052,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>1430</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="73" spans="1:76" x14ac:dyDescent="0.2">
@@ -13088,10 +13081,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>1431</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="74" spans="1:76" x14ac:dyDescent="0.2">
@@ -13117,10 +13110,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>1432</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="75" spans="1:76" x14ac:dyDescent="0.2">
@@ -13146,10 +13139,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>1433</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="76" spans="1:76" x14ac:dyDescent="0.2">
@@ -13175,10 +13168,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H76" s="2" t="s">
+        <v>1422</v>
+      </c>
+      <c r="K76" s="2" t="s">
         <v>1428</v>
-      </c>
-      <c r="K76" s="2" t="s">
-        <v>1434</v>
       </c>
     </row>
     <row r="77" spans="1:76" x14ac:dyDescent="0.2">
@@ -13204,10 +13197,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>1435</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="78" spans="1:76" x14ac:dyDescent="0.2">
@@ -13233,10 +13226,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>1436</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="79" spans="1:76" x14ac:dyDescent="0.2">
@@ -13262,10 +13255,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>1437</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="80" spans="1:76" x14ac:dyDescent="0.2">
@@ -13291,10 +13284,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>1438</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
@@ -13320,10 +13313,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>1439</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -13349,10 +13342,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>1440</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -13378,10 +13371,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>1441</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
@@ -13407,10 +13400,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>1442</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
@@ -13436,10 +13429,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>1443</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
@@ -13465,10 +13458,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>1444</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
@@ -13494,17 +13487,17 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>1445</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>3629700</v>
       </c>
-      <c r="B88" s="50">
+      <c r="B88" s="48">
         <v>1005283</v>
       </c>
       <c r="C88" s="2">
@@ -13523,10 +13516,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>1446</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
@@ -13552,10 +13545,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>1447</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
@@ -13581,10 +13574,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>1448</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
@@ -13610,10 +13603,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>1449</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
@@ -13639,10 +13632,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>1450</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
@@ -13668,10 +13661,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>1451</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
@@ -13697,10 +13690,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>1452</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
@@ -13726,10 +13719,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>1453</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
@@ -13755,10 +13748,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>1454</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
@@ -13784,10 +13777,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>1455</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
@@ -13813,10 +13806,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>1456</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
@@ -13842,10 +13835,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>1457</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
@@ -13871,10 +13864,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>1458</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
@@ -13900,10 +13893,10 @@
         <v>0.7895833333333333</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>1459</v>
+        <v>1453</v>
       </c>
     </row>
   </sheetData>
@@ -13918,8 +13911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC529FB-4C30-45A4-B2B2-CD6673B65124}">
   <dimension ref="A1:Q164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80:A113"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -14684,10 +14677,10 @@
       <c r="A20" s="2" t="s">
         <v>1110</v>
       </c>
-      <c r="B20" s="41">
+      <c r="B20" s="39">
         <v>3</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="40" t="s">
         <v>1151</v>
       </c>
       <c r="G20" s="4">
@@ -14725,10 +14718,10 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B21" s="43">
+      <c r="B21" s="41">
         <v>4</v>
       </c>
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="42" t="s">
         <v>1152</v>
       </c>
       <c r="G21" s="4">
@@ -14766,7 +14759,7 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="40">
+      <c r="B22" s="38">
         <v>10</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -14810,10 +14803,10 @@
       <c r="A23" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="B23" s="45">
+      <c r="B23" s="43">
         <v>7</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="44" t="s">
         <v>1154</v>
       </c>
       <c r="G23" s="4">
@@ -14852,7 +14845,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>1155</v>
+        <v>1455</v>
       </c>
       <c r="B24" s="1"/>
       <c r="G24" s="4">
@@ -14966,7 +14959,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>1156</v>
+        <v>1456</v>
       </c>
       <c r="B27" s="1"/>
       <c r="G27" s="4">
@@ -15073,7 +15066,7 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="45" t="s">
         <v>1112</v>
       </c>
       <c r="B30" s="1"/>
@@ -15218,7 +15211,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="G34" s="4">
         <v>211</v>
@@ -15254,7 +15247,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="G35" s="4">
         <v>213</v>
@@ -15290,7 +15283,7 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>1159</v>
+        <v>1459</v>
       </c>
       <c r="G36" s="4">
         <v>214</v>
@@ -15326,7 +15319,7 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>1160</v>
+        <v>1458</v>
       </c>
       <c r="G37" s="4">
         <v>216</v>
@@ -15364,7 +15357,7 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>1161</v>
+        <v>1457</v>
       </c>
       <c r="G38" s="4">
         <v>217</v>
@@ -15401,9 +15394,6 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>1162</v>
-      </c>
       <c r="G39" s="4">
         <v>220</v>
       </c>
@@ -15475,7 +15465,7 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>1163</v>
+        <v>1157</v>
       </c>
       <c r="G41" s="4">
         <v>223</v>
@@ -15511,7 +15501,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>1164</v>
+        <v>1158</v>
       </c>
       <c r="G42" s="4">
         <v>225</v>
@@ -15549,7 +15539,7 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>1165</v>
+        <v>1159</v>
       </c>
       <c r="G43" s="4">
         <v>229</v>
@@ -15587,7 +15577,7 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>1166</v>
+        <v>1160</v>
       </c>
       <c r="G44" s="4">
         <v>231</v>
@@ -15625,7 +15615,7 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>1167</v>
+        <v>1161</v>
       </c>
       <c r="G45" s="4">
         <v>232</v>
@@ -15663,7 +15653,7 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>1168</v>
+        <v>1162</v>
       </c>
       <c r="G46" s="4">
         <v>233</v>
@@ -15699,7 +15689,7 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>1169</v>
+        <v>1163</v>
       </c>
       <c r="G47" s="4">
         <v>234</v>
@@ -15737,7 +15727,7 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>1170</v>
+        <v>1164</v>
       </c>
       <c r="G48" s="4">
         <v>235</v>
@@ -15775,7 +15765,7 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>1171</v>
+        <v>1165</v>
       </c>
       <c r="G49" s="4">
         <v>236</v>
@@ -15813,7 +15803,7 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>1172</v>
+        <v>1166</v>
       </c>
       <c r="G50" s="4">
         <v>242</v>
@@ -15851,7 +15841,7 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>1173</v>
+        <v>1167</v>
       </c>
       <c r="G51" s="4">
         <v>243</v>
@@ -15889,7 +15879,7 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>1174</v>
+        <v>1168</v>
       </c>
       <c r="G52" s="4">
         <v>244</v>
@@ -15927,7 +15917,7 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>1175</v>
+        <v>1169</v>
       </c>
       <c r="G53" s="4">
         <v>246</v>
@@ -15965,7 +15955,7 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>1176</v>
+        <v>1170</v>
       </c>
       <c r="G54" s="4">
         <v>250</v>
@@ -16003,7 +15993,7 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>1177</v>
+        <v>1171</v>
       </c>
       <c r="G55" s="4">
         <v>251</v>
@@ -16041,7 +16031,7 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>1178</v>
+        <v>1172</v>
       </c>
       <c r="G56" s="4">
         <v>252</v>
@@ -16079,7 +16069,7 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>1179</v>
+        <v>1173</v>
       </c>
       <c r="G57" s="4">
         <v>253</v>
@@ -16117,7 +16107,7 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>1180</v>
+        <v>1174</v>
       </c>
       <c r="G58" s="4">
         <v>254</v>
@@ -16155,7 +16145,7 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>1181</v>
+        <v>1175</v>
       </c>
       <c r="G59" s="4">
         <v>269</v>
@@ -16193,7 +16183,7 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>1182</v>
+        <v>1176</v>
       </c>
       <c r="G60" s="4">
         <v>270</v>
@@ -16231,7 +16221,7 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>1183</v>
+        <v>1177</v>
       </c>
       <c r="G61" s="4">
         <v>277</v>
@@ -16269,7 +16259,7 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>1184</v>
+        <v>1178</v>
       </c>
       <c r="G62" s="4">
         <v>278</v>
@@ -16307,7 +16297,7 @@
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>1185</v>
+        <v>1179</v>
       </c>
       <c r="G63" s="4">
         <v>279</v>
@@ -16345,7 +16335,7 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>1186</v>
+        <v>1180</v>
       </c>
       <c r="G64" s="4">
         <v>280</v>
@@ -16383,7 +16373,7 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>1187</v>
+        <v>1181</v>
       </c>
       <c r="G65" s="4">
         <v>281</v>
@@ -16421,7 +16411,7 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>1188</v>
+        <v>1182</v>
       </c>
       <c r="G66" s="4">
         <v>282</v>
@@ -16459,7 +16449,7 @@
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>1189</v>
+        <v>1183</v>
       </c>
       <c r="G67" s="4">
         <v>283</v>
@@ -16497,7 +16487,7 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>1190</v>
+        <v>1184</v>
       </c>
       <c r="G68" s="4">
         <v>284</v>
@@ -16535,7 +16525,7 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>1191</v>
+        <v>1185</v>
       </c>
       <c r="G69" s="4">
         <v>285</v>
@@ -16573,7 +16563,7 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>1192</v>
+        <v>1186</v>
       </c>
       <c r="G70" s="4">
         <v>286</v>
@@ -16611,7 +16601,7 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>1193</v>
+        <v>1187</v>
       </c>
       <c r="G71" s="4">
         <v>287</v>
@@ -16649,7 +16639,7 @@
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>1194</v>
+        <v>1188</v>
       </c>
       <c r="G72" s="4">
         <v>288</v>
@@ -16687,7 +16677,7 @@
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>1195</v>
+        <v>1189</v>
       </c>
       <c r="G73" s="4">
         <v>289</v>
@@ -16725,7 +16715,7 @@
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>1196</v>
+        <v>1190</v>
       </c>
       <c r="G74" s="4">
         <v>290</v>
@@ -16763,7 +16753,7 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>1197</v>
+        <v>1191</v>
       </c>
       <c r="G75" s="4">
         <v>292</v>
@@ -16799,7 +16789,7 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>1198</v>
+        <v>1192</v>
       </c>
       <c r="G76" s="4">
         <v>295</v>
@@ -16837,7 +16827,7 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>1199</v>
+        <v>1193</v>
       </c>
       <c r="G77" s="4">
         <v>296</v>
@@ -16875,7 +16865,7 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>1200</v>
+        <v>1194</v>
       </c>
       <c r="G78" s="4">
         <v>297</v>
@@ -16948,7 +16938,7 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>1201</v>
+        <v>1195</v>
       </c>
       <c r="G80" s="4">
         <v>304</v>
@@ -16986,7 +16976,7 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>1202</v>
+        <v>1196</v>
       </c>
       <c r="G81" s="4">
         <v>315</v>
@@ -17022,7 +17012,7 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>1203</v>
+        <v>1197</v>
       </c>
       <c r="G82" s="4">
         <v>317</v>
@@ -17060,7 +17050,7 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>1204</v>
+        <v>1198</v>
       </c>
       <c r="G83" s="4">
         <v>318</v>
@@ -17098,7 +17088,7 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>1205</v>
+        <v>1199</v>
       </c>
       <c r="G84" s="4">
         <v>328</v>
@@ -17132,7 +17122,7 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>1206</v>
+        <v>1200</v>
       </c>
       <c r="G85" s="4">
         <v>329</v>
@@ -17166,7 +17156,7 @@
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>1207</v>
+        <v>1201</v>
       </c>
       <c r="G86" s="4">
         <v>332</v>
@@ -17200,7 +17190,7 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>1208</v>
+        <v>1202</v>
       </c>
       <c r="G87" s="4">
         <v>333</v>
@@ -17234,7 +17224,7 @@
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>1209</v>
+        <v>1203</v>
       </c>
       <c r="G88" s="4">
         <v>334</v>
@@ -17268,7 +17258,7 @@
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>1210</v>
+        <v>1204</v>
       </c>
       <c r="G89" s="4">
         <v>339</v>
@@ -17300,7 +17290,7 @@
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>1211</v>
+        <v>1205</v>
       </c>
       <c r="G90" s="4">
         <v>340</v>
@@ -17338,7 +17328,7 @@
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>1212</v>
+        <v>1206</v>
       </c>
       <c r="G91" s="4">
         <v>342</v>
@@ -17374,7 +17364,7 @@
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>1213</v>
+        <v>1207</v>
       </c>
       <c r="G92" s="4">
         <v>343</v>
@@ -17408,7 +17398,7 @@
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>1214</v>
+        <v>1208</v>
       </c>
       <c r="G93" s="4">
         <v>345</v>
@@ -17446,7 +17436,7 @@
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>1215</v>
+        <v>1209</v>
       </c>
       <c r="G94" s="4">
         <v>346</v>
@@ -17478,7 +17468,7 @@
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>1216</v>
+        <v>1210</v>
       </c>
       <c r="G95" s="4">
         <v>347</v>
@@ -17514,7 +17504,7 @@
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>1217</v>
+        <v>1211</v>
       </c>
       <c r="G96" s="4">
         <v>348</v>
@@ -17550,7 +17540,7 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>1218</v>
+        <v>1212</v>
       </c>
       <c r="G97" s="4">
         <v>368</v>
@@ -17582,7 +17572,7 @@
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>1219</v>
+        <v>1213</v>
       </c>
       <c r="G98" s="4">
         <v>369</v>
@@ -17614,7 +17604,7 @@
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>1220</v>
+        <v>1214</v>
       </c>
       <c r="G99" s="4">
         <v>375</v>
@@ -17650,7 +17640,7 @@
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>1221</v>
+        <v>1215</v>
       </c>
       <c r="G100" s="4">
         <v>376</v>
@@ -17682,7 +17672,7 @@
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>1222</v>
+        <v>1216</v>
       </c>
       <c r="G101" s="4">
         <v>378</v>
@@ -17718,7 +17708,7 @@
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>1223</v>
+        <v>1217</v>
       </c>
       <c r="G102" s="4">
         <v>380</v>
@@ -17750,7 +17740,7 @@
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>1224</v>
+        <v>1218</v>
       </c>
       <c r="G103" s="4">
         <v>381</v>
@@ -17782,7 +17772,7 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>1225</v>
+        <v>1219</v>
       </c>
       <c r="G104" s="4">
         <v>382</v>
@@ -17818,7 +17808,7 @@
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>1226</v>
+        <v>1220</v>
       </c>
       <c r="G105" s="4">
         <v>383</v>
@@ -17850,7 +17840,7 @@
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>1227</v>
+        <v>1221</v>
       </c>
       <c r="G106" s="4">
         <v>387</v>
@@ -17888,7 +17878,7 @@
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>1228</v>
+        <v>1222</v>
       </c>
       <c r="G107" s="4">
         <v>388</v>
@@ -17920,7 +17910,7 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>1229</v>
+        <v>1223</v>
       </c>
       <c r="G108" s="4">
         <v>389</v>
@@ -17952,7 +17942,7 @@
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>1230</v>
+        <v>1224</v>
       </c>
       <c r="G109" s="4">
         <v>390</v>
@@ -17990,7 +17980,7 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>1231</v>
+        <v>1225</v>
       </c>
       <c r="G110" s="4">
         <v>391</v>
@@ -18028,7 +18018,7 @@
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>1232</v>
+        <v>1226</v>
       </c>
       <c r="G111" s="4">
         <v>392</v>
@@ -18066,7 +18056,7 @@
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>1233</v>
+        <v>1227</v>
       </c>
       <c r="G112" s="4">
         <v>393</v>
@@ -18104,7 +18094,7 @@
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>1234</v>
+        <v>1228</v>
       </c>
       <c r="G113" s="4">
         <v>394</v>
@@ -33502,14 +33492,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="34"/>
-      <c r="C1" s="35" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="33" t="s">
         <v>1113</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="33" t="s">
         <v>1114</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="34" t="s">
         <v>1115</v>
       </c>
     </row>
@@ -33526,68 +33516,59 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="21"/>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="22" t="s">
         <v>1116</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="22" t="s">
         <v>1136</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="2:8" ht="10.8" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="18"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="21"/>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="4" t="s">
         <v>1117</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="4" t="s">
         <v>1118</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="22" t="s">
         <v>1119</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="22" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="22" t="s">
         <v>1121</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="22" t="s">
         <v>1122</v>
       </c>
       <c r="H12" s="17" t="s">
@@ -33596,65 +33577,55 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="22" t="s">
         <v>1123</v>
       </c>
-      <c r="H13" s="38" t="s">
+      <c r="H13" s="36" t="s">
         <v>1138</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="22" t="s">
         <v>1131</v>
       </c>
-      <c r="H14" s="38" t="s">
+      <c r="H14" s="36" t="s">
         <v>1139</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="22" t="s">
         <v>1124</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="H15" s="36" t="s">
         <v>1140</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="22" t="s">
         <v>1125</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="36" t="s">
         <v>1141</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="21"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="22" t="s">
         <v>1134</v>
       </c>
-      <c r="H17" s="38" t="s">
+      <c r="H17" s="36" t="s">
         <v>1143</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="24"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="29"/>
-      <c r="H18" s="38" t="s">
+      <c r="B18" s="23"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="28"/>
+      <c r="H18" s="36" t="s">
         <v>1145</v>
       </c>
     </row>
@@ -33666,140 +33637,129 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="18"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="30"/>
-      <c r="H20" s="37"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="29"/>
+      <c r="H20" s="35"/>
     </row>
     <row r="21" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B21" s="21"/>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="4" t="s">
         <v>1126</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="4" t="s">
         <v>1118</v>
       </c>
-      <c r="E21" s="31"/>
-      <c r="H21" s="39" t="s">
+      <c r="E21" s="30"/>
+      <c r="H21" s="37" t="s">
         <v>1146</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="21"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="5" t="s">
         <v>1127</v>
       </c>
-      <c r="E22" s="31"/>
+      <c r="E22" s="30"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="21"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="5" t="s">
         <v>1128</v>
       </c>
-      <c r="E23" s="31"/>
+      <c r="E23" s="30"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="21"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="5" t="s">
         <v>1129</v>
       </c>
-      <c r="E24" s="31"/>
+      <c r="E24" s="30"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="21"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="4" t="s">
         <v>1130</v>
       </c>
-      <c r="E25" s="31"/>
+      <c r="E25" s="30"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="21"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="5" t="s">
         <v>1132</v>
       </c>
-      <c r="E26" s="31"/>
+      <c r="E26" s="30"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="21"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="5" t="s">
         <v>1133</v>
       </c>
-      <c r="E27" s="31"/>
+      <c r="E27" s="30"/>
     </row>
     <row r="28" spans="2:8" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25"/>
     </row>
     <row r="29" spans="2:8" ht="10.8" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="18"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="28"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="27"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="21"/>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="4" t="s">
         <v>1135</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="4" t="s">
         <v>1118</v>
       </c>
-      <c r="E31" s="31"/>
+      <c r="E31" s="30"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="21"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="4" t="s">
         <v>1137</v>
       </c>
-      <c r="E32" s="31"/>
+      <c r="E32" s="30"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="21"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="32" t="s">
+      <c r="D33" s="5" t="s">
         <v>1132</v>
       </c>
-      <c r="E33" s="31"/>
+      <c r="E33" s="30"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="21"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="32" t="s">
+      <c r="D34" s="5" t="s">
         <v>1133</v>
       </c>
-      <c r="E34" s="31"/>
+      <c r="E34" s="30"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="21"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="32" t="s">
+      <c r="D35" s="5" t="s">
         <v>1128</v>
       </c>
-      <c r="E35" s="31"/>
+      <c r="E35" s="30"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="21"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="32" t="s">
+      <c r="D36" s="5" t="s">
         <v>1129</v>
       </c>
-      <c r="E36" s="31"/>
+      <c r="E36" s="30"/>
     </row>
     <row r="37" spans="2:5" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="24"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="26"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>